<commit_message>
Add digestion enzyme list
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/ms_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/ms_measurement_registration_sheet.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sven1103/git/data-manager/user-interface/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B9A8D5-1367-FE40-848A-922050B46DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685119FC-C364-4B45-B3B2-4B5566F52EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-5500" windowWidth="38400" windowHeight="23500" activeTab="2" xr2:uid="{D4F19D33-EE39-EF46-8DDD-2818EAD74D6D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{D4F19D33-EE39-EF46-8DDD-2818EAD74D6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
     <sheet name="Property information" sheetId="3" r:id="rId2"/>
     <sheet name="Allowed values" sheetId="2" r:id="rId3"/>
+    <sheet name="Digestion Method - Info" sheetId="4" r:id="rId4"/>
+    <sheet name="Digestion Enzyme - Info" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,8 +39,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="91">
   <si>
     <t>Measurement Property</t>
   </si>
@@ -155,13 +179,169 @@
   </si>
   <si>
     <t xml:space="preserve">number </t>
+  </si>
+  <si>
+    <t>see Digestion Method - Info</t>
+  </si>
+  <si>
+    <t>in gel</t>
+  </si>
+  <si>
+    <t>on beads</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Method </t>
+  </si>
+  <si>
+    <t>in solition</t>
+  </si>
+  <si>
+    <t>iST poteomics kit</t>
+  </si>
+  <si>
+    <t>see Digestion Enzyme - Info</t>
+  </si>
+  <si>
+    <t>BNPS-SKATOLE</t>
+  </si>
+  <si>
+    <t>CASPASE1</t>
+  </si>
+  <si>
+    <t>CASPASE2</t>
+  </si>
+  <si>
+    <t>CASPASE3</t>
+  </si>
+  <si>
+    <t>CASPASE4</t>
+  </si>
+  <si>
+    <t>CASPASE5</t>
+  </si>
+  <si>
+    <t>CASPASE6</t>
+  </si>
+  <si>
+    <t>CASPASE7</t>
+  </si>
+  <si>
+    <t>CASPASE8</t>
+  </si>
+  <si>
+    <t>CASPASE9</t>
+  </si>
+  <si>
+    <t>CASPASE10</t>
+  </si>
+  <si>
+    <t>CNBR</t>
+  </si>
+  <si>
+    <t>ENTEROKINASE</t>
+  </si>
+  <si>
+    <t>GRANZYMEB</t>
+  </si>
+  <si>
+    <t>HYDROXYLAMINE</t>
+  </si>
+  <si>
+    <t>NTCB</t>
+  </si>
+  <si>
+    <t>PEPSIN_LOW_PH</t>
+  </si>
+  <si>
+    <t>PEPSIN_HIGH_PH</t>
+  </si>
+  <si>
+    <t>PROLINE-ENDOPEPTIDASE</t>
+  </si>
+  <si>
+    <t>THERMOLYSIN</t>
+  </si>
+  <si>
+    <t>THROMBIN</t>
+  </si>
+  <si>
+    <t>FORMIC_ACID</t>
+  </si>
+  <si>
+    <t>STAPHYLOCOCCAL_PEPTIDASE_I</t>
+  </si>
+  <si>
+    <t>IODOSOBENZOIC_ACID</t>
+  </si>
+  <si>
+    <t>CLOSTRIPAIN:CLOSTRIDIOPEPTIDASE_B</t>
+  </si>
+  <si>
+    <t>TOBACCO_ETCH_VIRUS_PROTEASE</t>
+  </si>
+  <si>
+    <t>NEUTROPHIL_ELASTASE</t>
+  </si>
+  <si>
+    <t>PROTEINASE_K</t>
+  </si>
+  <si>
+    <t>FACTOR_XA</t>
+  </si>
+  <si>
+    <t>ASP-N_ENDOPEPTIDASE</t>
+  </si>
+  <si>
+    <t>ARG-C_PROTEINASE</t>
+  </si>
+  <si>
+    <t>ASP-N_ENDOPEPTIDASE_AND_N-TERMINAL_GLU</t>
+  </si>
+  <si>
+    <t>TRYPSIN</t>
+  </si>
+  <si>
+    <t>LYSC</t>
+  </si>
+  <si>
+    <t>LYSN</t>
+  </si>
+  <si>
+    <t>GLUTAMYL_ENDOPEPTIDASE</t>
+  </si>
+  <si>
+    <t>PNGASE_F</t>
+  </si>
+  <si>
+    <t>PAPAIN</t>
+  </si>
+  <si>
+    <t>IDEZ</t>
+  </si>
+  <si>
+    <t>IDES</t>
+  </si>
+  <si>
+    <t>IGDE</t>
+  </si>
+  <si>
+    <t>CHYMOTRYPSIN_LOW_SPECIFICITY</t>
+  </si>
+  <si>
+    <t>CHYMOTRYPSIN_HIGH_SPECIFICITY</t>
+  </si>
+  <si>
+    <t>CHYMOTRYPSIN</t>
+  </si>
+  <si>
+    <t>Enzyme code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -196,6 +376,19 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -217,7 +410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -227,6 +420,8 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,7 +759,7 @@
   <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:Q1"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -699,6 +894,18 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2D82C767-3EA1-B24E-9118-9B9604CF2E68}">
+          <x14:formula1>
+            <xm:f>'Digestion Method - Info'!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>G1:G1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -906,8 +1113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA9A15C-9427-F34B-B818-4D616E8AFF0A}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -918,7 +1125,7 @@
     <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.1640625" customWidth="1"/>
     <col min="8" max="8" width="22.83203125" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24" customWidth="1"/>
@@ -1001,10 +1208,10 @@
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H2" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="I2" t="s">
         <v>37</v>
@@ -1026,6 +1233,305 @@
         <v>13</v>
       </c>
       <c r="J4" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19673337-81F1-9E4F-81C7-A149B57EC048}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="8"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="8"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="8"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC23FEBF-A01A-EA46-8CE4-A566FF3483FE}">
+  <dimension ref="A1:B45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="e" cm="1">
+        <f t="array" ref="B2">SM</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>89</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>